<commit_message>
Excel generate output + JSON schema form
</commit_message>
<xml_diff>
--- a/shacl-play/src/main/webapp/theme-default/example/SHACL-template.xlsx
+++ b/shacl-play/src/main/webapp/theme-default/example/SHACL-template.xlsx
@@ -15,6 +15,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="0">#REF!</definedName>
   </definedNames>
   <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
@@ -318,13 +321,13 @@
     <t xml:space="preserve">Type of nodes that the values must have (ususally sh:IRI or sh:Literal)</t>
   </si>
   <si>
-    <t xml:space="preserve">For literal values, the expected datatype of the values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected class that the values of the predicate/path must have, if only one. If more than one, use sh:or</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If needed, expected shape that the values of the predicate/path must follow. This must be a reference to a URI of NodeShape from the first sheet</t>
+    <t xml:space="preserve">For literal values, the expected datatype of the values. If you put more than one, this will be automatically wrapped into a sh:or.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected class that the values of the predicate/path must have.  If you put more than one, this will be automatically wrapped into a sh:or.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If needed, expected shape that the values of the predicate/path must follow. This must be a reference to a URI of NodeShape from the first sheet.  If you put more than one, this will be automatically wrapped into a sh:or.</t>
   </si>
   <si>
     <t xml:space="preserve">The shape that must be verified by the qualifiedMin or qualifiedMax count</t>
@@ -393,13 +396,13 @@
     <t>sh:maxCount^^xsd:integer</t>
   </si>
   <si>
-    <t>sh:datatype</t>
-  </si>
-  <si>
-    <t>sh:class</t>
-  </si>
-  <si>
-    <t>sh:node</t>
+    <t xml:space="preserve">sh:datatype(separator="," wrapper="sh:or")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:class(separator="," wrapper="sh:or")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:node(separator="," wrapper="sh:or")</t>
   </si>
   <si>
     <t>sh:qualifiedValueShape</t>
@@ -491,11 +494,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="160" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* \-??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="161" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="162" formatCode="#"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* \-??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="#"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="27">
     <font>
       <sz val="10.000000"/>
       <color theme="1"/>
@@ -507,7 +510,6 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -518,7 +520,6 @@
     <font>
       <b/>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -546,17 +547,14 @@
     <font>
       <b/>
       <sz val="24.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="18.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -583,12 +581,6 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -601,7 +593,6 @@
       <i/>
       <u/>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -633,11 +624,6 @@
     <font>
       <b/>
       <sz val="10.000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.000000"/>
       <color indexed="4"/>
       <name val="Arial"/>
     </font>
@@ -876,7 +862,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="64"/>
         <bgColor rgb="FF393E45"/>
       </patternFill>
     </fill>
@@ -1150,16 +1135,16 @@
     </xf>
     <xf fontId="13" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="13" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="14" fillId="42" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1170,34 +1155,34 @@
     <xf fontId="16" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1209,13 +1194,13 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1239,10 +1224,10 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="18" fillId="42" borderId="2" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="19" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf fontId="17" fillId="42" borderId="2" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="16" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1251,19 +1236,19 @@
     <xf fontId="16" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="19" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf fontId="19" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="20" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="20" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
-    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="13" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="48">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="13" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
@@ -1275,64 +1260,50 @@
     <xf fontId="13" fillId="0" borderId="0" numFmtId="0" xfId="166" applyFont="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="166" applyFont="1" applyProtection="1">
+    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="166" applyFont="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+      <alignment wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="23" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="22" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+      <alignment wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="0">
+      <alignment wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="21" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="23" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="23" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="24" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="23" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="24" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="22" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="23" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="46" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="24" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="24" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="24" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="23" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="24" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="23" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1348,21 +1319,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="13" fillId="0" borderId="0" numFmtId="0" xfId="166" applyFont="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1377,14 +1333,11 @@
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="46" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1395,118 +1348,76 @@
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="46" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
+    <xf fontId="0" fillId="46" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="23" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="22" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="24" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="23" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="24" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="23" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="24" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="25" fillId="47" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="4" fillId="47" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="25" fillId="47" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="4" fillId="47" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="25" fillId="47" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="4" fillId="47" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="25" fillId="47" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="4" fillId="47" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="25" fillId="47" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="24" fillId="6" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="25" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="25" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="4" fillId="6" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="26" fillId="6" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="25" fillId="6" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="25" fillId="6" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="4" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="27" fillId="48" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="25" fillId="48" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="27" fillId="48" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="25" fillId="48" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="27" fillId="48" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="25" fillId="48" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="27" fillId="48" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="25" fillId="48" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="27" fillId="48" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="27" fillId="48" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="25" fillId="48" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="27" fillId="48" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="49" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="28" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="28" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="26" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="26" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2326,18 +2237,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" ht="12.75">
-      <c r="B16"/>
-      <c r="C16"/>
-    </row>
-    <row r="17" ht="12.75">
-      <c r="B17"/>
-      <c r="C17"/>
-    </row>
-    <row r="18" ht="12.75">
-      <c r="B18"/>
-      <c r="C18"/>
-    </row>
+    <row r="16" ht="12.75"/>
+    <row r="17" ht="12.75"/>
+    <row r="18" ht="12.75"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C1"/>
@@ -2464,7 +2366,6 @@
       <c r="I7" s="6"/>
     </row>
     <row r="8" ht="12.5">
-      <c r="C8"/>
       <c r="G8" s="8"/>
       <c r="I8" s="6"/>
     </row>
@@ -2489,133 +2390,131 @@
       <c r="AMD9" s="9"/>
     </row>
     <row r="10" s="9" customFormat="1" ht="12.5">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="K10" s="17"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="K10" s="12"/>
       <c r="N10" s="9"/>
-      <c r="ALZ10" s="14"/>
-      <c r="AMA10" s="14"/>
-      <c r="AMB10" s="14"/>
-      <c r="AMC10" s="14"/>
-      <c r="AMD10" s="14"/>
+      <c r="ALZ10" s="9"/>
+      <c r="AMA10" s="9"/>
+      <c r="AMB10" s="9"/>
+      <c r="AMC10" s="9"/>
+      <c r="AMD10" s="9"/>
     </row>
     <row r="11" ht="12.5">
-      <c r="A11"/>
-      <c r="B11"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" s="18" customFormat="1" ht="89.25" customHeight="1">
-      <c r="A12" s="18" t="s">
+    <row r="12" s="14" customFormat="1" ht="89.25" customHeight="1">
+      <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="M12" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
     </row>
     <row r="13" ht="44.700000000000003" customHeight="1">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="M13" s="24" t="s">
+      <c r="M13" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" ht="76.5">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="6" t="s">
         <v>75</v>
       </c>
       <c r="F14" t="s">
@@ -2628,28 +2527,28 @@
       <c r="I14" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="K14" s="30" t="s">
+      <c r="K14" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="M14" s="31"/>
+      <c r="M14" s="23"/>
     </row>
     <row r="15" ht="12.5">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="6" t="s">
         <v>83</v>
       </c>
       <c r="F15" t="s">
@@ -2662,10 +2561,10 @@
       <c r="I15" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="K15" s="30" t="s">
+      <c r="K15" s="22" t="s">
         <v>86</v>
       </c>
       <c r="L15" s="6" t="s">
@@ -2676,32 +2575,23 @@
       </c>
     </row>
     <row r="16" ht="12.75">
-      <c r="B16"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="K16" s="6"/>
     </row>
     <row r="17" ht="12.75">
-      <c r="A17"/>
-      <c r="B17"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
     <row r="18" ht="12.75">
-      <c r="A18"/>
-      <c r="B18"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" ht="12.75">
-      <c r="E19"/>
-    </row>
-    <row r="20" ht="12.75">
-      <c r="E20"/>
-    </row>
+    <row r="19" ht="12.75"/>
+    <row r="20" ht="12.75"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B1"/>
@@ -2741,22 +2631,20 @@
     <col customWidth="1" min="1" max="1" style="0" width="19.309999999999999"/>
     <col customWidth="1" min="2" max="2" style="6" width="41.450000000000003"/>
     <col customWidth="1" min="3" max="3" style="0" width="42.670000000000002"/>
-    <col customWidth="1" min="4" max="4" style="32" width="26.780000000000001"/>
+    <col customWidth="1" min="4" max="4" style="24" width="26.780000000000001"/>
     <col customWidth="1" min="5" max="5" style="6" width="41.450000000000003"/>
-    <col customWidth="1" min="6" max="6" style="31" width="41.090000000000003"/>
-    <col customWidth="1" min="7" max="7" style="33" width="14.539999999999999"/>
-    <col customWidth="1" min="8" max="8" style="34" width="11.99"/>
+    <col customWidth="1" min="6" max="6" style="23" width="41.090000000000003"/>
+    <col customWidth="1" min="7" max="7" style="25" width="14.539999999999999"/>
+    <col customWidth="1" min="8" max="8" style="26" width="11.99"/>
     <col customWidth="1" min="9" max="9" style="0" width="20.109999999999999"/>
-    <col customWidth="1" min="10" max="10" style="0" width="20.98"/>
-    <col customWidth="1" min="11" max="11" style="35" width="20.98"/>
+    <col customWidth="1" min="10" max="11" style="3" width="20.98"/>
     <col customWidth="1" min="12" max="12" style="0" width="27.57421875"/>
     <col customWidth="1" hidden="1" min="13" max="15" style="0" width="26"/>
-    <col customWidth="1" min="16" max="16" style="35" width="34.32"/>
+    <col customWidth="1" min="16" max="16" style="3" width="34.32"/>
     <col customWidth="1" hidden="1" min="17" max="17" style="0" width="36"/>
     <col customWidth="1" hidden="1" min="18" max="18" style="0" width="34.859999999999999"/>
     <col customWidth="1" min="19" max="19" width="34.859999999999999"/>
-    <col customWidth="1" min="20" max="20" style="6" width="28.109999999999999"/>
-    <col customWidth="1" min="21" max="21" style="6" width="28.109999999999999"/>
+    <col customWidth="1" min="20" max="21" style="6" width="28.109999999999999"/>
     <col customWidth="1" min="1020" max="1024" style="0" width="11.539999999999999"/>
   </cols>
   <sheetData>
@@ -2768,12 +2656,12 @@
         <v>32</v>
       </c>
       <c r="C1" s="6"/>
-      <c r="K1" s="35"/>
-      <c r="P1" s="27"/>
+      <c r="K1" s="3"/>
+      <c r="P1" s="6"/>
       <c r="S1" s="6"/>
     </row>
     <row r="2" ht="12.75">
-      <c r="K2" s="35"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" s="9" customFormat="1" ht="12.800000000000001">
       <c r="A3" s="10" t="s">
@@ -2781,19 +2669,19 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="36"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="14"/>
+      <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
-      <c r="P3" s="14"/>
+      <c r="P3" s="9"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
       <c r="S3" s="9"/>
@@ -2807,214 +2695,214 @@
       <c r="AMJ3" s="9"/>
     </row>
     <row r="4" ht="24" customHeight="1">
-      <c r="D4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="K4" s="35"/>
+      <c r="D4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="K4" s="3"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" s="19" customFormat="1" ht="76.5">
-      <c r="A5" s="19" t="s">
+    <row r="5" s="15" customFormat="1" ht="102">
+      <c r="A5" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="O5" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="P5" s="43" t="s">
+      <c r="P5" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="Q5" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="R5" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="S5" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="T5" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="U5" s="43" t="s">
+      <c r="U5" s="15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="6" s="44" customFormat="1" ht="25.5">
-      <c r="A6" s="44" t="s">
+    <row r="6" s="34" customFormat="1" ht="25.5">
+      <c r="A6" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="K6" s="48"/>
-      <c r="M6" s="44"/>
-      <c r="P6" s="48"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="K6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="P6" s="34"/>
     </row>
     <row r="7" ht="38.25">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="53" t="s">
+      <c r="G7" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="50" t="s">
+      <c r="J7" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="K7" s="54" t="s">
+      <c r="K7" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="M7" s="50" t="s">
+      <c r="M7" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="N7" s="50" t="s">
+      <c r="N7" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="O7" s="50" t="s">
+      <c r="O7" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="P7" s="54" t="s">
+      <c r="P7" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="Q7" s="22" t="s">
+      <c r="Q7" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="R7" s="50" t="s">
+      <c r="R7" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="S7" s="50" t="s">
+      <c r="S7" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="T7" s="50" t="s">
+      <c r="T7" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="U7" s="50" t="s">
+      <c r="U7" s="19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" s="55" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A8" s="55" t="s">
+    <row r="8" s="40" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A8" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="K8" s="59"/>
-      <c r="M8" s="55"/>
-      <c r="P8" s="60"/>
-      <c r="T8" s="61"/>
-      <c r="U8" s="60"/>
+      <c r="D8" s="41"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="K8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="P8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44"/>
     </row>
     <row r="9" ht="12.800000000000001">
-      <c r="A9" s="62" t="str">
+      <c r="A9" s="45" t="str">
         <f>CONCATENATE("example:P",ROW(A9))</f>
         <v>example:P9</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C9" t="s">
         <v>135</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="25">
         <v>1</v>
       </c>
-      <c r="H9" s="34">
+      <c r="H9" s="26">
         <v>1</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="46" t="s">
         <v>138</v>
       </c>
       <c r="J9" t="s">
         <v>139</v>
       </c>
-      <c r="K9" s="35"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" ht="12.800000000000001">
-      <c r="A10" s="62" t="str">
-        <f>CONCATENATE("example:P",ROW(A10))</f>
+      <c r="A10" s="45" t="str">
+        <f t="shared" ref="A10:A14" si="0">CONCATENATE("example:P",ROW(A10))</f>
         <v>example:P10</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -3023,29 +2911,29 @@
       <c r="C10" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="25">
         <v>1</v>
       </c>
-      <c r="H10" s="34">
+      <c r="H10" s="26">
         <v>1</v>
       </c>
-      <c r="I10" s="64" t="s">
+      <c r="I10" s="46" t="s">
         <v>138</v>
       </c>
       <c r="J10" t="s">
         <v>139</v>
       </c>
-      <c r="K10" s="35"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" ht="12.800000000000001">
-      <c r="A11" s="62" t="str">
-        <f>CONCATENATE("example:P",ROW(A11))</f>
+      <c r="A11" s="45" t="str">
+        <f t="shared" si="0"/>
         <v>example:P11</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -3054,43 +2942,42 @@
       <c r="C11" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="24" t="s">
         <v>144</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="64" t="s">
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="J11"/>
-      <c r="K11" s="65" t="s">
+      <c r="K11" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" s="55" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A12" s="55" t="s">
+    <row r="12" s="40" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A12" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="55"/>
-      <c r="K12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="61"/>
-      <c r="U12" s="60"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="44"/>
     </row>
     <row r="13" ht="12.800000000000001">
-      <c r="A13" s="62" t="str">
-        <f>CONCATENATE("example:P",ROW(A13))</f>
+      <c r="A13" s="45" t="str">
+        <f t="shared" si="0"/>
         <v>example:P13</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -3099,36 +2986,36 @@
       <c r="C13" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="25">
         <v>1</v>
       </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="67" t="s">
+      <c r="H13" s="26"/>
+      <c r="I13" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K13" s="35"/>
-      <c r="T13" s="25" t="s">
+      <c r="K13" s="3"/>
+      <c r="T13" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="U13" s="28" t="s">
+      <c r="U13" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" ht="12.800000000000001">
-      <c r="A14" s="62" t="str">
-        <f>CONCATENATE("example:P",ROW(A14))</f>
+      <c r="A14" s="45" t="str">
+        <f t="shared" si="0"/>
         <v>example:P14</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -3137,160 +3024,104 @@
       <c r="C14" t="s">
         <v>152</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34">
+      <c r="G14" s="25"/>
+      <c r="H14" s="26">
         <v>1</v>
       </c>
-      <c r="I14" s="64" t="s">
+      <c r="I14" s="46" t="s">
         <v>138</v>
       </c>
       <c r="J14" t="s">
         <v>139</v>
       </c>
-      <c r="K14" s="35"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" ht="12.75">
-      <c r="A15"/>
       <c r="B15" s="6"/>
-      <c r="C15"/>
-      <c r="D15" s="32"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15" s="35"/>
+      <c r="D15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="K15" s="3"/>
       <c r="T15" s="6"/>
     </row>
     <row r="16" ht="12.75">
-      <c r="A16"/>
       <c r="B16" s="6"/>
-      <c r="C16"/>
-      <c r="D16" s="32"/>
-      <c r="I16"/>
-      <c r="K16" s="35"/>
-      <c r="M16"/>
-      <c r="Q16"/>
+      <c r="D16" s="24"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" ht="12.75">
-      <c r="A17"/>
       <c r="B17" s="6"/>
-      <c r="C17"/>
-      <c r="D17" s="32"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17" s="35"/>
-      <c r="L17"/>
-      <c r="M17"/>
-      <c r="N17"/>
-      <c r="O17"/>
-      <c r="P17" s="35"/>
-      <c r="Q17"/>
-      <c r="R17"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="K17" s="3"/>
+      <c r="P17" s="3"/>
       <c r="T17" s="6"/>
-      <c r="AMJ17"/>
     </row>
     <row r="18" ht="12.75">
-      <c r="A18"/>
       <c r="B18" s="6"/>
-      <c r="C18"/>
-      <c r="D18" s="32"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
-      <c r="I18"/>
-      <c r="K18" s="35"/>
-      <c r="M18"/>
+      <c r="D18" s="24"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="K18" s="3"/>
       <c r="U18" s="6"/>
     </row>
     <row r="19" ht="12.75">
-      <c r="A19"/>
       <c r="B19" s="6"/>
-      <c r="C19"/>
-      <c r="D19" s="32"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19" s="35"/>
-      <c r="M19"/>
+      <c r="D19" s="24"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" ht="12.75">
-      <c r="A20"/>
       <c r="B20" s="6"/>
-      <c r="C20"/>
-      <c r="D20" s="32"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="34"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20" s="35"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20"/>
-      <c r="P20" s="35"/>
-      <c r="Q20"/>
-      <c r="R20"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="K20" s="3"/>
+      <c r="P20" s="3"/>
       <c r="T20" s="6"/>
-      <c r="AMJ20"/>
     </row>
     <row r="21" ht="12.75">
-      <c r="A21"/>
       <c r="B21" s="6"/>
-      <c r="C21"/>
-      <c r="D21" s="32"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="34"/>
-      <c r="I21"/>
-      <c r="K21" s="35"/>
-      <c r="M21"/>
+      <c r="D21" s="24"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="K21" s="3"/>
       <c r="U21" s="6"/>
     </row>
     <row r="22" ht="12.75">
-      <c r="A22"/>
       <c r="B22" s="6"/>
-      <c r="C22"/>
-      <c r="D22" s="32"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="34"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22" s="35"/>
-      <c r="M22"/>
+      <c r="D22" s="24"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="K22" s="3"/>
       <c r="T22" s="6"/>
     </row>
     <row r="23" ht="12.75">
-      <c r="A23"/>
-      <c r="K23" s="35"/>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" ht="12.75">
-      <c r="A24"/>
-      <c r="K24" s="35"/>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" ht="12.75">
-      <c r="K25" s="35"/>
-      <c r="M25"/>
+      <c r="K25" s="3"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" ht="12.75">
-      <c r="A26"/>
-    </row>
-    <row r="27" ht="12.75">
-      <c r="A27"/>
-    </row>
+    <row r="26" ht="12.75"/>
+    <row r="27" ht="12.75"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B1"/>

</xml_diff>